<commit_message>
Upload Y3_B2526_Biochemistry_LAB_CBL_System_2025-10-10T00-40-09.xlsx via attendance app
</commit_message>
<xml_diff>
--- a/log_history/Y3_B2526_Biochemistry_LAB_CBL_System_2025-10-10T00-40-09.xlsx
+++ b/log_history/Y3_B2526_Biochemistry_LAB_CBL_System_2025-10-10T00-40-09.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\Desktop\log_history\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F840BE-1DBE-4F7F-BCC4-C4EC63FAD46D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E82389-571D-4881-A6CF-30D159B830C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="10980" windowHeight="13770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1520" yWindow="580" windowWidth="18280" windowHeight="13100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1452,7 +1452,7 @@
     <t>System</t>
   </si>
   <si>
-    <t xml:space="preserve">Biochemistry Lab/CBL </t>
+    <t>Biochemistry LAB/CBL</t>
   </si>
 </sst>
 </file>
@@ -1802,7 +1802,7 @@
   <dimension ref="A1:F479"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>